<commit_message>
Verified Ready tc's WV-416, skip tc2-issue with locators, WV-544 Automation complete, no issues
</commit_message>
<xml_diff>
--- a/tests/browserstack_automation/testData/statesandcandidates.xlsx
+++ b/tests/browserstack_automation/testData/statesandcandidates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
   <si>
     <t>stateName</t>
   </si>
@@ -22,6 +22,9 @@
     <t>stateURL</t>
   </si>
   <si>
+    <t>stateAbb</t>
+  </si>
+  <si>
     <t>stateTitle</t>
   </si>
   <si>
@@ -31,6 +34,9 @@
     <t>alaska-candidates/cs/</t>
   </si>
   <si>
+    <t>AK</t>
+  </si>
+  <si>
     <t>Alaska Candidates - WeVote</t>
   </si>
   <si>
@@ -40,6 +46,9 @@
     <t>alabama-candidates/cs/</t>
   </si>
   <si>
+    <t>AL</t>
+  </si>
+  <si>
     <t>Alabama Candidates - WeVote</t>
   </si>
   <si>
@@ -49,6 +58,9 @@
     <t>arkansas-candidates/cs/</t>
   </si>
   <si>
+    <t>AR</t>
+  </si>
+  <si>
     <t>Arkansas Candidates - WeVote</t>
   </si>
   <si>
@@ -58,6 +70,9 @@
     <t>arizona-candidates/cs/</t>
   </si>
   <si>
+    <t>AZ</t>
+  </si>
+  <si>
     <t>Arizona Candidates - WeVote</t>
   </si>
   <si>
@@ -67,6 +82,9 @@
     <t>california-candidates/cs/</t>
   </si>
   <si>
+    <t>CA</t>
+  </si>
+  <si>
     <t>California Candidates - WeVote</t>
   </si>
   <si>
@@ -76,6 +94,9 @@
     <t>colorado-candidates/cs/</t>
   </si>
   <si>
+    <t>CO</t>
+  </si>
+  <si>
     <t>Colorado Candidates - WeVote</t>
   </si>
   <si>
@@ -85,6 +106,9 @@
     <t>connecticut-candidates/cs/</t>
   </si>
   <si>
+    <t>CT</t>
+  </si>
+  <si>
     <t>Connecticut Candidates - WeVote</t>
   </si>
   <si>
@@ -94,6 +118,9 @@
     <t>district-of-columbia-candidates/cs/</t>
   </si>
   <si>
+    <t>DC</t>
+  </si>
+  <si>
     <t>District of Columbia Candidates - WeVote</t>
   </si>
   <si>
@@ -103,6 +130,9 @@
     <t>delaware-candidates/cs/</t>
   </si>
   <si>
+    <t>DE</t>
+  </si>
+  <si>
     <t>Delaware Candidates - WeVote</t>
   </si>
   <si>
@@ -112,6 +142,9 @@
     <t>florida-candidates/cs/</t>
   </si>
   <si>
+    <t>FL</t>
+  </si>
+  <si>
     <t>Florida Candidates - WeVote</t>
   </si>
   <si>
@@ -121,6 +154,9 @@
     <t>georgia-candidates/cs/</t>
   </si>
   <si>
+    <t>GA</t>
+  </si>
+  <si>
     <t>Georgia Candidates - WeVote</t>
   </si>
   <si>
@@ -130,6 +166,9 @@
     <t>hawaii-candidates/cs/</t>
   </si>
   <si>
+    <t>HI</t>
+  </si>
+  <si>
     <t>Hawaii Candidates - WeVote</t>
   </si>
   <si>
@@ -139,6 +178,9 @@
     <t>iowa-candidates/cs/</t>
   </si>
   <si>
+    <t>IA</t>
+  </si>
+  <si>
     <t>Iowa Candidates - WeVote</t>
   </si>
   <si>
@@ -148,6 +190,9 @@
     <t>idaho-candidates/cs/</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>Idaho Candidates - WeVote</t>
   </si>
   <si>
@@ -157,6 +202,9 @@
     <t>illinois-candidates/cs/</t>
   </si>
   <si>
+    <t>IL</t>
+  </si>
+  <si>
     <t>Illinois Candidates - WeVote</t>
   </si>
   <si>
@@ -166,6 +214,9 @@
     <t>indiana-candidates/cs/</t>
   </si>
   <si>
+    <t>IN</t>
+  </si>
+  <si>
     <t>Indiana Candidates - WeVote</t>
   </si>
   <si>
@@ -175,6 +226,9 @@
     <t>kansas-candidates/cs/</t>
   </si>
   <si>
+    <t>KS</t>
+  </si>
+  <si>
     <t>Kansas Candidates - WeVote</t>
   </si>
   <si>
@@ -184,6 +238,9 @@
     <t>kentucky-candidates/cs/</t>
   </si>
   <si>
+    <t>KY</t>
+  </si>
+  <si>
     <t>Kentucky Candidates - WeVote</t>
   </si>
   <si>
@@ -193,6 +250,9 @@
     <t>louisiana-candidates/cs/</t>
   </si>
   <si>
+    <t>LA</t>
+  </si>
+  <si>
     <t>Louisiana Candidates - WeVote</t>
   </si>
   <si>
@@ -202,6 +262,9 @@
     <t>massachusetts-candidates/cs/</t>
   </si>
   <si>
+    <t>MA</t>
+  </si>
+  <si>
     <t>Massachusetts Candidates - WeVote</t>
   </si>
   <si>
@@ -211,6 +274,9 @@
     <t>maryland-candidates/cs/</t>
   </si>
   <si>
+    <t>MD</t>
+  </si>
+  <si>
     <t>Maryland Candidates - WeVote</t>
   </si>
   <si>
@@ -220,6 +286,9 @@
     <t>maine-candidates/cs/</t>
   </si>
   <si>
+    <t>ME</t>
+  </si>
+  <si>
     <t>Maine Candidates - WeVote</t>
   </si>
   <si>
@@ -229,6 +298,9 @@
     <t>michigan-candidates/cs/</t>
   </si>
   <si>
+    <t>MI</t>
+  </si>
+  <si>
     <t>Michigan Candidates - WeVote</t>
   </si>
   <si>
@@ -238,6 +310,9 @@
     <t>minnesota-candidates/cs/</t>
   </si>
   <si>
+    <t>MN</t>
+  </si>
+  <si>
     <t>Minnesota Candidates - WeVote</t>
   </si>
   <si>
@@ -247,6 +322,9 @@
     <t>montana-candidates/cs/</t>
   </si>
   <si>
+    <t>MT</t>
+  </si>
+  <si>
     <t>Montana Candidates - WeVote</t>
   </si>
   <si>
@@ -256,6 +334,9 @@
     <t>national-candidates/cs/</t>
   </si>
   <si>
+    <t>all</t>
+  </si>
+  <si>
     <t>Candidates - WeVote</t>
   </si>
   <si>
@@ -265,6 +346,9 @@
     <t>north-carolina-candidates/cs/</t>
   </si>
   <si>
+    <t>NC</t>
+  </si>
+  <si>
     <t>North Carolina Candidates - WeVote</t>
   </si>
   <si>
@@ -274,6 +358,9 @@
     <t>north-dakota-candidates/cs/</t>
   </si>
   <si>
+    <t>ND</t>
+  </si>
+  <si>
     <t>North Dakota Candidates - WeVote</t>
   </si>
   <si>
@@ -283,6 +370,9 @@
     <t>nebraska-candidates/cs/</t>
   </si>
   <si>
+    <t>NE</t>
+  </si>
+  <si>
     <t>Nebraska Candidates - WeVote</t>
   </si>
   <si>
@@ -292,6 +382,9 @@
     <t>new-hampshire-candidates/cs/</t>
   </si>
   <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>New Hampshire Candidates - WeVote</t>
   </si>
   <si>
@@ -301,6 +394,9 @@
     <t>new-jersey-candidates/cs/</t>
   </si>
   <si>
+    <t>NJ</t>
+  </si>
+  <si>
     <t>New Jersey Candidates - WeVote</t>
   </si>
   <si>
@@ -310,6 +406,9 @@
     <t>new-mexico-candidates/cs/</t>
   </si>
   <si>
+    <t>NM</t>
+  </si>
+  <si>
     <t>New Mexico Candidates - WeVote</t>
   </si>
   <si>
@@ -319,6 +418,9 @@
     <t>nevada-candidates/cs/</t>
   </si>
   <si>
+    <t>NV</t>
+  </si>
+  <si>
     <t>Nevada Candidates - WeVote</t>
   </si>
   <si>
@@ -328,6 +430,9 @@
     <t>new-york-candidates/cs/</t>
   </si>
   <si>
+    <t>NY</t>
+  </si>
+  <si>
     <t>New York Candidates - WeVote</t>
   </si>
   <si>
@@ -337,6 +442,9 @@
     <t>ohio-candidates/cs/</t>
   </si>
   <si>
+    <t>OH</t>
+  </si>
+  <si>
     <t>Ohio Candidates - WeVote</t>
   </si>
   <si>
@@ -346,6 +454,9 @@
     <t>oklahoma-candidates/cs/</t>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
     <t>Oklahoma Candidates - WeVote</t>
   </si>
   <si>
@@ -355,6 +466,9 @@
     <t>oregon-candidates/cs/</t>
   </si>
   <si>
+    <t>OR</t>
+  </si>
+  <si>
     <t>Oregon Candidates - WeVote</t>
   </si>
   <si>
@@ -364,6 +478,9 @@
     <t>pennsylvania-candidates/cs/</t>
   </si>
   <si>
+    <t>PA</t>
+  </si>
+  <si>
     <t>Pennsylvania Candidates - WeVote</t>
   </si>
   <si>
@@ -373,6 +490,9 @@
     <t>rhode-island-candidates/cs/</t>
   </si>
   <si>
+    <t>RI</t>
+  </si>
+  <si>
     <t>Rhode Island Candidates - WeVote</t>
   </si>
   <si>
@@ -382,6 +502,9 @@
     <t>south-carolina-candidates/cs/</t>
   </si>
   <si>
+    <t>SC</t>
+  </si>
+  <si>
     <t>South Carolina Candidates - WeVote</t>
   </si>
   <si>
@@ -391,6 +514,9 @@
     <t>south-dakota-candidates/cs/</t>
   </si>
   <si>
+    <t>SD</t>
+  </si>
+  <si>
     <t>South Dakota Candidates - WeVote</t>
   </si>
   <si>
@@ -400,6 +526,9 @@
     <t>tennessee-candidates/cs/</t>
   </si>
   <si>
+    <t>TN</t>
+  </si>
+  <si>
     <t>Tennessee Candidates - WeVote</t>
   </si>
   <si>
@@ -409,6 +538,9 @@
     <t>texas-candidates/cs/</t>
   </si>
   <si>
+    <t>TX</t>
+  </si>
+  <si>
     <t>Texas Candidates - WeVote</t>
   </si>
   <si>
@@ -418,6 +550,9 @@
     <t>utah-candidates/cs/</t>
   </si>
   <si>
+    <t>UT</t>
+  </si>
+  <si>
     <t>Utah Candidates - WeVote</t>
   </si>
   <si>
@@ -427,6 +562,9 @@
     <t>virginia-candidates/cs/</t>
   </si>
   <si>
+    <t>VA</t>
+  </si>
+  <si>
     <t>Virginia Candidates - WeVote</t>
   </si>
   <si>
@@ -436,6 +574,9 @@
     <t>vermont-candidates/cs/</t>
   </si>
   <si>
+    <t>VT</t>
+  </si>
+  <si>
     <t>Vermont Candidates - WeVote</t>
   </si>
   <si>
@@ -445,6 +586,9 @@
     <t>washington-candidates/cs/</t>
   </si>
   <si>
+    <t>WA</t>
+  </si>
+  <si>
     <t>Washington Candidates - WeVote</t>
   </si>
   <si>
@@ -454,6 +598,9 @@
     <t>wisconsin-candidates/cs/</t>
   </si>
   <si>
+    <t>WI</t>
+  </si>
+  <si>
     <t>Wisconsin Candidates - WeVote</t>
   </si>
   <si>
@@ -463,6 +610,9 @@
     <t>west-virginia-candidates/cs/</t>
   </si>
   <si>
+    <t>WV</t>
+  </si>
+  <si>
     <t>West Virginia Candidates - WeVote</t>
   </si>
   <si>
@@ -470,6 +620,9 @@
   </si>
   <si>
     <t>wyoming-candidates/cs/</t>
+  </si>
+  <si>
+    <t>WY</t>
   </si>
   <si>
     <t>Wyoming Candidates - WeVote</t>
@@ -490,7 +643,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -522,9 +675,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -832,576 +991,730 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="29.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="43.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="40.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="43.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="40.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>89</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>97</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>101</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>80</v>
+        <v>105</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>83</v>
+        <v>109</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>86</v>
+        <v>113</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>92</v>
+        <v>121</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>95</v>
+        <v>125</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>98</v>
+        <v>129</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>101</v>
+        <v>133</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>104</v>
+        <v>137</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>107</v>
+        <v>141</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>149</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>116</v>
+        <v>153</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>119</v>
+        <v>157</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>122</v>
+        <v>161</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>125</v>
+        <v>165</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="1" t="s">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>128</v>
+        <v>169</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="1" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>134</v>
+        <v>177</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>137</v>
+        <v>181</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="1" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>140</v>
+        <v>185</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="1" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>143</v>
+        <v>189</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="1" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>146</v>
+        <v>193</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="1" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>149</v>
+        <v>197</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="1" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>152</v>
+        <v>201</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>